<commit_message>
Added 2-nd KE lab + title
</commit_message>
<xml_diff>
--- a/2 course/ElectricalEngineering/2/Calc.xlsx
+++ b/2 course/ElectricalEngineering/2/Calc.xlsx
@@ -3,12 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5F499F-0895-40A6-8A2A-1A08F4273F11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFC16A8-2271-4D4B-ABA5-795EFDAF219A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Schem1" sheetId="2" r:id="rId2"/>
+    <sheet name="Schem2" sheetId="3" r:id="rId3"/>
+    <sheet name="Result" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t>Var</t>
   </si>
@@ -43,13 +46,154 @@
   </si>
   <si>
     <t>R3</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R1+R3</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R2+R3</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>I11</t>
+  </si>
+  <si>
+    <t>I22</t>
+  </si>
+  <si>
+    <t>(E1-I22*R12)/R11</t>
+  </si>
+  <si>
+    <t>(E2+R12*I11)/R2</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>I1+I2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>I1*R1</t>
+  </si>
+  <si>
+    <t>I2*R2</t>
+  </si>
+  <si>
+    <t>I3*R3</t>
+  </si>
+  <si>
+    <t>Self check</t>
+  </si>
+  <si>
+    <t>U1+U3</t>
+  </si>
+  <si>
+    <t>U2+U3</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PE2</t>
+  </si>
+  <si>
+    <t>PE1+PE2</t>
+  </si>
+  <si>
+    <t>I1*E1</t>
+  </si>
+  <si>
+    <t>I2*E2</t>
+  </si>
+  <si>
+    <t>PR1</t>
+  </si>
+  <si>
+    <t>PR2</t>
+  </si>
+  <si>
+    <t>PR3</t>
+  </si>
+  <si>
+    <t>I1*U1</t>
+  </si>
+  <si>
+    <t>I2*U2</t>
+  </si>
+  <si>
+    <t>I3*U3</t>
+  </si>
+  <si>
+    <t>PR1+PR2+PR3</t>
+  </si>
+  <si>
+    <t>Excpected</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>U2-U3</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,16 +207,31 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -80,11 +239,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -93,11 +387,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,12 +1087,12 @@
         <f>L1</f>
         <v>Var</v>
       </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="I8" s="5">
+        <v>3</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -819,23 +1155,23 @@
       </c>
       <c r="H10" s="3">
         <f ca="1">INDIRECT(_xlfn.CONCAT("B",I8+1))</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="I10" s="3">
         <f ca="1">INDIRECT(_xlfn.CONCAT("C",I8+1))</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J10" s="3">
         <f ca="1">INDIRECT(_xlfn.CONCAT("D",I8+1))</f>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="K10" s="3">
         <f ca="1">INDIRECT(_xlfn.CONCAT("E",I8+1))</f>
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L10" s="3">
         <f ca="1">INDIRECT(_xlfn.CONCAT("F",I8+1))</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -858,7 +1194,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -982,7 +1318,7 @@
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1008,7 +1344,7 @@
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -1367,4 +1703,802 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B593086-0D8A-4B42-8B2C-E74A2D549878}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7">
+        <f ca="1">Data!H10</f>
+        <v>60</v>
+      </c>
+      <c r="G2" s="13">
+        <f ca="1">C11+C13</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13">
+        <f ca="1">Data!J10+Data!L10</f>
+        <v>70</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="7">
+        <f ca="1">Data!I10</f>
+        <v>60</v>
+      </c>
+      <c r="G3" s="13">
+        <f ca="1">C12+C13</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13">
+        <f ca="1">Data!K10+Data!L10</f>
+        <v>75</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="13">
+        <f ca="1">C8*Data!H10</f>
+        <v>40.824742268041241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13">
+        <f ca="1">Data!L10</f>
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="13">
+        <f ca="1">C9*Data!I10</f>
+        <v>37.113402061855673</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="13">
+        <f ca="1">(Data!H10-Schem1!C7*Schem1!C5)/Schem1!C3</f>
+        <v>0.68041237113402064</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="13">
+        <f ca="1">G5+G4</f>
+        <v>77.938144329896915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="13">
+        <f ca="1">(Schem1!C3*Data!I10-Schem1!C5*Data!H10)/(C4*C3-C5*C5)</f>
+        <v>0.61855670103092786</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="13">
+        <f ca="1">C8*Schem1!C11</f>
+        <v>23.148049739611011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13">
+        <f ca="1">C6</f>
+        <v>0.68041237113402064</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="13">
+        <f ca="1">C9*C12</f>
+        <v>21.043681581464558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="13">
+        <f ca="1">C7</f>
+        <v>0.61855670103092786</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="13">
+        <f ca="1">C10*C13</f>
+        <v>33.746413008821342</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13">
+        <f ca="1">C8+C9</f>
+        <v>1.2989690721649485</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="16">
+        <f ca="1">G6</f>
+        <v>77.938144329896915</v>
+      </c>
+      <c r="G10" s="17">
+        <f ca="1">SUM(G7:G9)</f>
+        <v>77.938144329896915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="13">
+        <f ca="1">C8*Data!J10</f>
+        <v>34.020618556701031</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="13">
+        <f ca="1">C9*Data!K10</f>
+        <v>34.020618556701031</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="17">
+        <f ca="1">C10*Data!L10</f>
+        <v>25.979381443298969</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E531CBA-78B3-4709-B82C-C31A47FB7C17}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7">
+        <f ca="1">Data!H10</f>
+        <v>60</v>
+      </c>
+      <c r="G2" s="13">
+        <f ca="1">C11+C13</f>
+        <v>60.000000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13">
+        <f ca="1">Data!J10+Data!L10</f>
+        <v>70</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="7">
+        <f ca="1">Data!I10</f>
+        <v>60</v>
+      </c>
+      <c r="G3" s="13">
+        <f ca="1">C12-C13</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13">
+        <f ca="1">Data!K10+Data!L10</f>
+        <v>75</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="13">
+        <f ca="1">C8*F2</f>
+        <v>70.515463917525778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13">
+        <f ca="1">Data!L10</f>
+        <v>20</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="13">
+        <f ca="1">F3*C9</f>
+        <v>66.80412371134021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="13">
+        <f ca="1">(Data!H10+Schem2!C7*Schem2!C5)/Schem2!C3</f>
+        <v>1.1752577319587629</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="13">
+        <f ca="1">G5+G4</f>
+        <v>137.31958762886597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="13">
+        <f ca="1">(Schem1!C3*Data!I10+Schem1!C5*Data!H10)/(C4*C3-C5*C5)</f>
+        <v>1.1134020618556701</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="13">
+        <f ca="1">C8*C11</f>
+        <v>69.061536826442776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13">
+        <f ca="1">C6</f>
+        <v>1.1752577319587629</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="13">
+        <f ca="1">C9*C12</f>
+        <v>68.181528323945159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="13">
+        <f ca="1">C7</f>
+        <v>1.1134020618556701</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="13">
+        <f ca="1">C10*C13</f>
+        <v>7.6522478478052935E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13">
+        <f ca="1">C8-C9</f>
+        <v>6.1855670103092786E-2</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="16">
+        <f ca="1">G6</f>
+        <v>137.31958762886597</v>
+      </c>
+      <c r="G10" s="17">
+        <f ca="1">SUM(G7:G9)</f>
+        <v>137.31958762886597</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="13">
+        <f ca="1">C8*Data!J10</f>
+        <v>58.762886597938149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="13">
+        <f ca="1">C9*Data!K10</f>
+        <v>61.237113402061858</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="17">
+        <f ca="1">C10*Data!L10</f>
+        <v>1.2371134020618557</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86D247B-ED67-4690-9075-577155056B0B}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="6">
+        <f ca="1">Data!H10</f>
+        <v>60</v>
+      </c>
+      <c r="C2" s="6">
+        <f ca="1">Data!I10</f>
+        <v>60</v>
+      </c>
+      <c r="D2" s="6">
+        <f t="array" aca="1" ref="D2:E2" ca="1">TRANSPOSE(Schem1!G4:G5)</f>
+        <v>40.824742268041241</v>
+      </c>
+      <c r="E2" s="6">
+        <f ca="1"/>
+        <v>37.113402061855673</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="array" aca="1" ref="F2:H2" ca="1">TRANSPOSE(Schem1!G7:G9)</f>
+        <v>23.148049739611011</v>
+      </c>
+      <c r="G2" s="6">
+        <f ca="1"/>
+        <v>21.043681581464558</v>
+      </c>
+      <c r="H2" s="6">
+        <f ca="1"/>
+        <v>33.746413008821342</v>
+      </c>
+      <c r="I2" s="6">
+        <f ca="1">D2+E2</f>
+        <v>77.938144329896915</v>
+      </c>
+      <c r="J2" s="6">
+        <f ca="1">F2+G2+H2</f>
+        <v>77.938144329896915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6">
+        <f ca="1">B2</f>
+        <v>60</v>
+      </c>
+      <c r="C3" s="6">
+        <f ca="1">C2</f>
+        <v>60</v>
+      </c>
+      <c r="D3" s="6">
+        <f ca="1">D2</f>
+        <v>40.824742268041241</v>
+      </c>
+      <c r="E3" s="6">
+        <f ca="1">E2</f>
+        <v>37.113402061855673</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:H3" ca="1" si="0">F2</f>
+        <v>23.148049739611011</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>21.043681581464558</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>33.746413008821342</v>
+      </c>
+      <c r="I3" s="6">
+        <f t="shared" ref="I3" ca="1" si="1">I2</f>
+        <v>77.938144329896915</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3" ca="1" si="2">J2</f>
+        <v>77.938144329896915</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="str">
+        <f>A2</f>
+        <v>Measured</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" ref="B4:C7" ca="1" si="3">B3</f>
+        <v>60</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" ca="1" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="array" aca="1" ref="D4:E4" ca="1">TRANSPOSE(Schem2!G4:G5)</f>
+        <v>70.515463917525778</v>
+      </c>
+      <c r="E4" s="6">
+        <f ca="1"/>
+        <v>66.80412371134021</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="array" aca="1" ref="F4:H4" ca="1">TRANSPOSE(Schem2!G7:G9)</f>
+        <v>69.061536826442776</v>
+      </c>
+      <c r="G4" s="6">
+        <f ca="1"/>
+        <v>68.181528323945159</v>
+      </c>
+      <c r="H4" s="6">
+        <f ca="1"/>
+        <v>7.6522478478052935E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="array" aca="1" ref="I4:J4" ca="1">TRANSPOSE(Schem2!G4:G5)</f>
+        <v>70.515463917525778</v>
+      </c>
+      <c r="J4" s="6">
+        <f ca="1"/>
+        <v>66.80412371134021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="str">
+        <f t="shared" ref="A5:A7" si="4">A3</f>
+        <v>Calculated</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" ca="1" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" ca="1" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="D5" s="6">
+        <f ca="1">D4</f>
+        <v>70.515463917525778</v>
+      </c>
+      <c r="E5" s="6">
+        <f ca="1">E4</f>
+        <v>66.80412371134021</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:H5" ca="1" si="5">F4</f>
+        <v>69.061536826442776</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>68.181528323945159</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.6522478478052935E-2</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" ref="I5" ca="1" si="6">I4</f>
+        <v>70.515463917525778</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" ref="J5" ca="1" si="7">J4</f>
+        <v>66.80412371134021</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>